<commit_message>
Actualizaci├│n de c├│digo y preguntas
</commit_message>
<xml_diff>
--- a/preguntas.xlsx
+++ b/preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01 academico\001 Doctorado Economia UCAB\d tesis problema ahorro\5.4 experimentos\cuestionario\proyecto_encuesta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CDE198-854B-4578-AE78-99C1B0E8B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD8C140-A947-467A-BF01-9A46176EFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{951E78D8-AB70-4378-8378-F124DB33DEFF}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Prefiero evitar perder $100 que ganar $200.</t>
   </si>
   <si>
-    <t>likert</t>
-  </si>
-  <si>
     <t>1: Totalmente en desacuerdo, 2: En desacuerdo, 3: Neutral, 4: De acuerdo, 5: Totalmente de acuerdo</t>
   </si>
   <si>
@@ -88,22 +85,22 @@
     <t>A menudo asigno mi dinero a categorías específicas (por ejemplo, ‘para diversión’, ‘para ahorro’, ‘para emergencias’) y evito usarlo para otros fines, incluso si fuera más lógico o beneficioso hacerlo</t>
   </si>
   <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>pregunta</t>
-  </si>
-  <si>
-    <t>escala</t>
-  </si>
-  <si>
-    <t>posibles respuestas</t>
-  </si>
-  <si>
-    <t>Binario</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1: De acuerdo, 2: Totalmente de acuerdo</t>
+  </si>
+  <si>
+    <t>1: SI, 2: NO, 3: NO SE</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>PREGUNTA</t>
+  </si>
+  <si>
+    <t>ESCALA</t>
+  </si>
+  <si>
+    <t>POSIBLES_RESPUESTAS</t>
   </si>
 </sst>
 </file>
@@ -972,30 +969,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A896E8D-0727-4477-AAF2-6FF9BCA79489}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="94.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="88.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,11 +1002,11 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="C2">
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1017,13 +1014,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1031,13 +1028,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,13 +1042,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,13 +1056,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,13 +1070,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
         <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,13 +1084,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,13 +1098,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,13 +1112,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1129,13 +1126,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,13 +1140,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,13 +1154,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,13 +1168,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,13 +1182,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,13 +1196,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,13 +1210,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,13 +1224,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,13 +1238,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,13 +1252,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,13 +1266,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>